<commit_message>
Applied data driven with excel for Stack linked list and modified background
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhavya\eclipse-workspace\bug_busters\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00745188-926C-47C6-9DC7-8BE4E898AAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D004C24C-C1B8-4605-AF10-F73C9953387F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>username</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>hello</t>
+  </si>
+  <si>
+    <t>Hii</t>
+  </si>
+  <si>
+    <t>NameError: name 'Hii' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>NameError: empty not accepted</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -427,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -501,7 +513,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9941EEDA-BEDA-4CE1-91EF-BD56BF58E9FE}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
@@ -510,7 +522,7 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -535,6 +547,22 @@
       </c>
       <c r="B3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -584,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85E9C1C-BBB4-4198-80D6-0F550928EBF1}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Updated sheet for Editor (changed Alert Message)
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhavya\eclipse-workspace\bug_busters\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D004C24C-C1B8-4605-AF10-F73C9953387F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DB45618C-EFF4-4942-8B22-0BA5E3495BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,8 @@
     <sheet name="Background" sheetId="3" r:id="rId3"/>
     <sheet name="Linkedlist" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:J5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,9 +65,6 @@
     <t>Hello</t>
   </si>
   <si>
-    <t>AlertMessage</t>
-  </si>
-  <si>
     <t>print("Hello")</t>
   </si>
   <si>
@@ -103,6 +96,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>NameError: name 'Hello' is not defined on line 1</t>
   </si>
 </sst>
 </file>
@@ -516,7 +512,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -538,12 +534,12 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -551,18 +547,18 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -624,26 +620,26 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
         <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Applied data driven with excel for Try Editor page of Data Structure!
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -17,17 +17,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1742018138" val="1064" rev="124" rev64="64" revOS="1" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1742018138" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1742018138" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1742018138"/>
+      <pm:revision xmlns:pm="smNativeData" day="1742140250" val="1064" rev="124" rev64="64" revOS="1" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1742140250" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1742140250" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1742140250"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
   <si>
     <t>username</t>
   </si>
@@ -74,6 +74,18 @@
     <t>print("Hello")</t>
   </si>
   <si>
+    <t>Hii</t>
+  </si>
+  <si>
+    <t>NameError: name 'Hii' is not defined on line 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>NameError: empty not accepted</t>
+  </si>
+  <si>
     <t>UserInputCode</t>
   </si>
   <si>
@@ -98,13 +110,7 @@
     <t>password2</t>
   </si>
   <si>
-    <t>Register@Numpy</t>
-  </si>
-  <si>
-    <t>Reg_Bugbusters</t>
-  </si>
-  <si>
-    <t>New Account Created. You are logged in as</t>
+    <t>Please fill in this field.</t>
   </si>
   <si>
     <t>Numpy_Testers</t>
@@ -125,8 +131,13 @@
     <t>bug@12</t>
   </si>
   <si>
-    <t xml:space="preserve">password_mismatch:The two password fields didn’t match.
-</t>
+    <t>DSAlgo@Application</t>
+  </si>
+  <si>
+    <t>DSALGO@Bugbusters</t>
+  </si>
+  <si>
+    <t>New Account Created. You are logged in as DSAlgo@Application</t>
   </si>
 </sst>
 </file>
@@ -151,7 +162,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742018138" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -166,7 +177,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742018138" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -181,7 +192,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742018138" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" ulstyle="none" kern="1">
             <pm:latin face="Arial Unicode MS" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -197,7 +208,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742018138" fgClr="0563C1" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" fgClr="0563C1" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -213,7 +224,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742018138" fgClr="0563C1" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" fgClr="0563C1" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -229,7 +240,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742018138" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -252,7 +263,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1742018138" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1742140250" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -274,7 +285,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1742018138"/>
+          <pm:border xmlns:pm="smNativeData" id="1742140250"/>
         </ext>
       </extLst>
     </border>
@@ -293,7 +304,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1742018138"/>
+          <pm:border xmlns:pm="smNativeData" id="1742140250"/>
         </ext>
       </extLst>
     </border>
@@ -302,16 +313,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -322,10 +330,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1742018138" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1742140250" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1742018138" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1742140250" count="1">
         <pm:color name="Color 24" rgb="0563C1"/>
       </pm:colors>
     </ext>
@@ -592,7 +600,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
@@ -662,7 +670,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742018138" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742140250" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -671,14 +679,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742018138" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742018138" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742018138" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742140250" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -689,7 +697,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
@@ -698,7 +706,7 @@
   <sheetFormatPr defaultRowHeight="15.40"/>
   <cols>
     <col min="1" max="1" width="13.723214" customWidth="1"/>
-    <col min="2" max="2" width="13.544643" customWidth="1"/>
+    <col min="2" max="2" width="39.366071" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -725,11 +733,27 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742018138" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742140250" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -738,14 +762,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742018138" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742018138" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742018138" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742140250" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -759,12 +783,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
   <cols>
-    <col min="2" max="2" width="10.366071" customWidth="1"/>
+    <col min="1" max="1" width="11.821429" customWidth="1"/>
+    <col min="2" max="2" width="13.116071" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -790,7 +815,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742018138" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742140250" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -799,14 +824,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742018138" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742018138" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742018138" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742140250" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -820,44 +845,44 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
   <cols>
-    <col min="1" max="1" width="13.455357" customWidth="1"/>
+    <col min="1" max="1" width="15.267857" customWidth="1"/>
     <col min="2" max="2" width="39.089286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742018138" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742140250" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -866,14 +891,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742018138" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742018138" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742018138" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742140250" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -887,15 +912,15 @@
   <dimension ref="A1:XFD9"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="15.40"/>
   <cols>
-    <col min="1" max="1" width="19.241071" customWidth="1" style="5"/>
-    <col min="2" max="2" width="17.901786" customWidth="1" style="5"/>
-    <col min="3" max="3" width="20.651786" customWidth="1" style="5"/>
-    <col min="4" max="4" width="58.553571" customWidth="1" style="5"/>
+    <col min="1" max="1" width="19.125000" customWidth="1" style="5"/>
+    <col min="2" max="2" width="19.366071" customWidth="1" style="5"/>
+    <col min="3" max="3" width="23.866071" customWidth="1" style="5"/>
+    <col min="4" max="4" width="58.348214" customWidth="1" style="5"/>
     <col min="5" max="16384" width="10.000000" style="5"/>
   </cols>
   <sheetData>
@@ -904,117 +929,114 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>24</v>
-      </c>
+    <row r="2" spans="4:4">
       <c r="D2" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D3" s="5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>27</v>
+      <c r="B6" s="5" t="n">
+        <v>12345678</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>12345678</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>12345678</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>12345678</v>
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="5" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2:C2" r:id="rId1"/>
-  </hyperlinks>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742018138" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742140250" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1023,14 +1045,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742018138" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742018138" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742018138" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742140250" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Background Data Driven implemented !
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -5,29 +5,30 @@
   <fileSharing readOnlyRecommended="0" userName="balasahebshendkar"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="4" xWindow="240" yWindow="60" windowWidth="19418" windowHeight="10298" tabRatio="500"/>
+    <workbookView activeTab="5" xWindow="240" yWindow="60" windowWidth="19418" windowHeight="11498" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId4"/>
     <sheet name="Editor" sheetId="2" r:id="rId5"/>
-    <sheet name="Background" sheetId="3" r:id="rId6"/>
-    <sheet name="Linkedlist" sheetId="4" r:id="rId7"/>
-    <sheet name="Register" sheetId="5" r:id="rId8"/>
+    <sheet name="Array" sheetId="3" r:id="rId6"/>
+    <sheet name="Background" sheetId="4" r:id="rId7"/>
+    <sheet name="Linkedlist" sheetId="5" r:id="rId8"/>
+    <sheet name="Register" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1742140250" val="1064" rev="124" rev64="64" revOS="1" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1742140250" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1742140250" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1742140250"/>
+      <pm:revision xmlns:pm="smNativeData" day="1742236693" val="1064" rev="124" rev64="64" revOS="1" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1742236693" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1742236693" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1742236693"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
   <si>
     <t>username</t>
   </si>
@@ -68,7 +69,7 @@
     <t>Hello</t>
   </si>
   <si>
-    <t>AlertMessage</t>
+    <t>NameError: name 'Hello' is not defined on line 1</t>
   </si>
   <si>
     <t>print("Hello")</t>
@@ -86,6 +87,120 @@
     <t>NameError: empty not accepted</t>
   </si>
   <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>ExpectedOutput</t>
+  </si>
+  <si>
+    <t>Search The Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def search(input_list, num):
+     return num in input_list
+input_list = [12, 23, 45, 67, 6, 90]
+num = 11
+if search(input_list, num):
+    print("Element Found".format(num))
+else:
+    print("Element Not Found".format(num))
+    </t>
+  </si>
+  <si>
+    <t>Element Not Found</t>
+  </si>
+  <si>
+    <t>Invalid Code</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>Submission Successful</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t>Find Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    max_count = 0
+    current_count = 0
+    for num in nums:
+        if num == 1:
+            current_count += 1
+            max_count = max(max_count, current_count)
+        else:
+            current_count = 0
+    return max_count
+binary_array = [1, 1, 0, 1, 1, 1, 0, 1]
+result = findMaxConsecutiveOnes(binary_array)
+print(result)</t>
+  </si>
+  <si>
+    <t>Even Number of Digits</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+    def is_even_digit_number(n):
+        return len(str(abs(n))) % 2 == 0
+    count = 0
+    for num in nums:
+        if is_even_digit_number(num):
+            count += 1
+    return count
+nums = [12, 345, 2, 6, 7896, 24]
+result = findNumbers(nums)
+print(result)</t>
+  </si>
+  <si>
+    <t>Squares of a Sorted Array</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+    left = 0
+    right = len(nums) - 1
+    result = [0] * len(nums)
+    index = len(nums) - 1
+    while left &lt;= right:
+        left_square = nums[left] ** 2
+        right_square = nums[right] ** 2
+        if left_square &gt; right_square:
+            result[index] = left_square
+            left += 1
+        else:
+            result[index] = right_square
+            right -= 1
+        index -= 1
+    return result
+nums = [-4, -1, 0, 3, 10]
+result = sortedSquares(nums)
+print(result)</t>
+  </si>
+  <si>
+    <t>[0, 1, 9, 16, 100]</t>
+  </si>
+  <si>
+    <t>Try Editor</t>
+  </si>
+  <si>
+    <t>print("VALID CODE")</t>
+  </si>
+  <si>
+    <t>VALID CODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INVALID </t>
+  </si>
+  <si>
+    <t>NameError: name 'INVALID' is not defined on line 1</t>
+  </si>
+  <si>
     <t>UserInputCode</t>
   </si>
   <si>
@@ -129,22 +244,13 @@
   </si>
   <si>
     <t>bug@12</t>
-  </si>
-  <si>
-    <t>DSAlgo@Application</t>
-  </si>
-  <si>
-    <t>DSALGO@Bugbusters</t>
-  </si>
-  <si>
-    <t>New Account Created. You are logged in as DSAlgo@Application</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="5" formatCode="#,##0\ &quot;₹&quot;;\-#,##0\ &quot;₹&quot;"/>
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;₹&quot;;[Red]\-#,##0\ &quot;₹&quot;"/>
     <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;₹&quot;;\-#,##0.00\ &quot;₹&quot;"/>
@@ -153,6 +259,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0\ _₹_-;\-* #,##0\ _₹_-;_-* &quot;-&quot;\ _₹_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₹&quot;_-;\-* #,##0.00\ &quot;₹&quot;_-;_-* &quot;-&quot;??\ &quot;₹&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₹_-;\-* #,##0.00\ _₹_-;_-* &quot;-&quot;??\ _₹_-;_-@_-"/>
+    <numFmt numFmtId="1" formatCode="0"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -162,7 +269,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -177,7 +284,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -192,7 +299,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" ulstyle="none" kern="1">
             <pm:latin face="Arial Unicode MS" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -208,7 +315,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" fgClr="0563C1" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" fgClr="0563C1" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -224,7 +331,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" fgClr="0563C1" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" fgClr="0563C1" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -240,7 +347,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742140250" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -250,26 +357,15 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1742140250" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -285,26 +381,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1742140250"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1742140250"/>
+          <pm:border xmlns:pm="smNativeData" id="1742236693"/>
         </ext>
       </extLst>
     </border>
@@ -313,15 +390,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -330,10 +408,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1742140250" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1742236693" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1742140250" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1742236693" count="1">
         <pm:color name="Color 24" rgb="0563C1"/>
       </pm:colors>
     </ext>
@@ -635,7 +713,7 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
@@ -670,7 +748,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742140250" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -679,14 +757,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742140250" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -700,13 +778,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
   <cols>
     <col min="1" max="1" width="13.723214" customWidth="1"/>
-    <col min="2" max="2" width="39.366071" customWidth="1"/>
+    <col min="2" max="2" width="40.455357" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -753,7 +831,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742140250" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -762,14 +840,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742140250" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -780,42 +858,233 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView view="normal" topLeftCell="A7" zoomScale="60" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
   <cols>
-    <col min="1" max="1" width="11.821429" customWidth="1"/>
-    <col min="2" max="2" width="13.116071" customWidth="1"/>
+    <col min="1" max="1" width="23.901786" customWidth="1"/>
+    <col min="2" max="2" width="33.812500" customWidth="1"/>
+    <col min="3" max="3" width="43.901786" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742140250" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -824,14 +1093,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742140250" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -842,47 +1111,41 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.40"/>
   <cols>
-    <col min="1" max="1" width="15.267857" customWidth="1"/>
-    <col min="2" max="2" width="39.089286" customWidth="1"/>
+    <col min="2" max="2" width="10.366071" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742140250" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -891,14 +1154,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742140250" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -909,134 +1172,192 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:XFD9"/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.40"/>
+  <cols>
+    <col min="1" max="1" width="13.455357" customWidth="1"/>
+    <col min="2" max="2" width="39.089286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.700000" right="0.700000" top="0.750000" bottom="0.750000" header="0.300000" footer="0.300000"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="15.40"/>
   <cols>
-    <col min="1" max="1" width="19.125000" customWidth="1" style="5"/>
-    <col min="2" max="2" width="19.366071" customWidth="1" style="5"/>
-    <col min="3" max="3" width="23.866071" customWidth="1" style="5"/>
-    <col min="4" max="4" width="58.348214" customWidth="1" style="5"/>
-    <col min="5" max="16384" width="10.000000" style="5"/>
+    <col min="1" max="1" width="21.517857" customWidth="1"/>
+    <col min="2" max="2" width="21.919643" customWidth="1"/>
+    <col min="3" max="3" width="26.205357" customWidth="1"/>
+    <col min="4" max="4" width="54.464286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="4:4">
-      <c r="D2" s="5" t="s">
-        <v>27</v>
+      <c r="D2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>27</v>
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>27</v>
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>31</v>
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="5" t="n">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="n">
         <v>12345678</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" t="n">
         <v>12345678</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>31</v>
+      <c r="D6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>31</v>
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>31</v>
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742140250" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1045,14 +1366,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742140250" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742140250" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Trying to resolve conflict !
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -18,10 +18,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1742236693" val="1064" rev="124" rev64="64" revOS="1" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1742236693" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1742236693" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1742236693"/>
+      <pm:revision xmlns:pm="smNativeData" day="1742243006" val="1064" rev="124" rev64="64" revOS="1" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1742243006" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1742243006" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1742243006"/>
     </ext>
   </extLst>
 </workbook>
@@ -240,7 +240,7 @@
     <t>password_mismatch:The two password fields didn’t match.</t>
   </si>
   <si>
-    <t>Bug@Busters</t>
+    <t>Team_Bug@busters</t>
   </si>
   <si>
     <t>bug@12</t>
@@ -269,7 +269,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742243006" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -284,7 +284,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742243006" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -299,7 +299,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742243006" ulstyle="none" kern="1">
             <pm:latin face="Arial Unicode MS" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -315,7 +315,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" fgClr="0563C1" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742243006" fgClr="0563C1" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -331,7 +331,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" fgClr="0563C1" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742243006" fgClr="0563C1" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -347,7 +347,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1742236693" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1742243006" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -357,15 +357,26 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1742243006" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -381,7 +392,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1742236693"/>
+          <pm:border xmlns:pm="smNativeData" id="1742243006"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1742243006"/>
         </ext>
       </extLst>
     </border>
@@ -408,10 +438,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1742236693" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1742243006" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1742236693" count="1">
+      <pm:colors xmlns:pm="smNativeData" id="1742243006" count="1">
         <pm:color name="Color 24" rgb="0563C1"/>
       </pm:colors>
     </ext>
@@ -748,7 +778,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742243006" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -757,14 +787,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742243006" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -831,7 +861,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742243006" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -840,14 +870,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742243006" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1084,7 +1114,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742243006" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1093,14 +1123,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742243006" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1145,7 +1175,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742243006" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1154,14 +1184,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742243006" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1212,7 +1242,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742243006" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1221,14 +1251,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742243006" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1242,7 +1272,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="15.40"/>
@@ -1324,7 +1354,7 @@
         <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
         <v>54</v>
@@ -1357,7 +1387,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1742236693" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1742243006" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1366,14 +1396,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1742236693" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1742243006" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742236693" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1742243006" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Updated Linked list with data driven and updated a bug at Home page
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhavya\eclipse-workspace\bug_busters\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DC4D2D-91B8-4416-B4A1-283AAE16D329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA5AEF7-A22D-403A-87C4-53E6CB6A530A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="58">
   <si>
     <t>username</t>
   </si>
@@ -242,6 +242,15 @@
   <si>
     <t xml:space="preserve">New Account Created. You are logged in as Bug@Ninjas
 </t>
+  </si>
+  <si>
+    <t>expectedOutputType</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t>Console</t>
   </si>
 </sst>
 </file>
@@ -666,7 +675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552CCD6A-B613-482B-AF9E-AB5B0F15B42E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -802,56 +811,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9941EEDA-BEDA-4CE1-91EF-BD56BF58E9FE}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.453125" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Register - Expected Result
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -3,18 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DB45618C-EFF4-4942-8B22-0BA5E3495BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0E463EA0-CC69-4FE8-9AAD-A49B481C4D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Editor" sheetId="2" r:id="rId2"/>
-    <sheet name="Background" sheetId="3" r:id="rId3"/>
-    <sheet name="Linkedlist" sheetId="4" r:id="rId4"/>
+    <sheet name="Register" sheetId="6" r:id="rId2"/>
+    <sheet name="Editor" sheetId="2" r:id="rId3"/>
+    <sheet name="Array" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J5"/>
+  <oleSize ref="A1:N8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="53">
   <si>
     <t>username</t>
   </si>
@@ -68,24 +68,6 @@
     <t>print("Hello")</t>
   </si>
   <si>
-    <t>UserInputCode</t>
-  </si>
-  <si>
-    <t>ExpectedResult</t>
-  </si>
-  <si>
-    <t>hii</t>
-  </si>
-  <si>
-    <t>NameError: name 'hii' is not defined on line 1</t>
-  </si>
-  <si>
-    <t>print 'hello'</t>
-  </si>
-  <si>
-    <t>hello</t>
-  </si>
-  <si>
     <t>Hii</t>
   </si>
   <si>
@@ -98,14 +80,165 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>ExpectedOutput</t>
+  </si>
+  <si>
+    <t xml:space="preserve">def search(input_list, num):
+     return num in input_list
+input_list = [12, 23, 45, 67, 6, 90]
+num = 11
+if search(input_list, num):
+    print("Element Found".format(num))
+else:
+    print("Element Not Found".format(num))
+    </t>
+  </si>
+  <si>
+    <t>Element Not Found</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>Invalid Code</t>
+  </si>
+  <si>
+    <t>Search The Array</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Submission Successful</t>
+  </si>
+  <si>
+    <t>Error occurred during submission</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums):
+    max_count = 0
+    current_count = 0
+    for num in nums:
+        if num == 1:
+            current_count += 1
+            max_count = max(max_count, current_count)
+        else:
+            current_count = 0
+    return max_count
+binary_array = [1, 1, 0, 1, 1, 1, 0, 1]
+result = findMaxConsecutiveOnes(binary_array)
+print(result)</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):
+    def is_even_digit_number(n):
+        return len(str(abs(n))) % 2 == 0
+    count = 0
+    for num in nums:
+        if is_even_digit_number(num):
+            count += 1
+    return count
+nums = [12, 345, 2, 6, 7896, 24]
+result = findNumbers(nums)
+print(result)</t>
+  </si>
+  <si>
+    <t>Even Number of Digits</t>
+  </si>
+  <si>
+    <t>Find Max Consecutive Ones</t>
+  </si>
+  <si>
+    <t>def sortedSquares(nums):
+    left = 0
+    right = len(nums) - 1
+    result = [0] * len(nums)
+    index = len(nums) - 1
+    while left &lt;= right:
+        left_square = nums[left] ** 2
+        right_square = nums[right] ** 2
+        if left_square &gt; right_square:
+            result[index] = left_square
+            left += 1
+        else:
+            result[index] = right_square
+            right -= 1
+        index -= 1
+    return result
+nums = [-4, -1, 0, 3, 10]
+result = sortedSquares(nums)
+print(result)</t>
+  </si>
+  <si>
+    <t>Squares of a Sorted Array</t>
+  </si>
+  <si>
+    <t>[0, 1, 9, 16, 100]</t>
+  </si>
+  <si>
+    <t>Try Editor</t>
+  </si>
+  <si>
+    <t>print("VALID CODE")</t>
+  </si>
+  <si>
+    <t>VALID CODE</t>
+  </si>
+  <si>
+    <t>NameError: name 'INVALID' is not defined on line 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INVALID </t>
+  </si>
+  <si>
     <t>NameError: name 'Hello' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>password2</t>
+  </si>
+  <si>
+    <t>Numpy_Testers</t>
+  </si>
+  <si>
+    <t>Bug_Busters</t>
+  </si>
+  <si>
+    <t>*Numpy&amp;Testers*</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>TeamBug@busters</t>
+  </si>
+  <si>
+    <t>Team@busters</t>
+  </si>
+  <si>
+    <t>bug@12</t>
+  </si>
+  <si>
+    <t>Bug@Ninjas</t>
+  </si>
+  <si>
+    <t>Ninjas@Testers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Account Created. You are logged in as Bug@Ninjas
+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +255,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,10 +288,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -435,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="60" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -508,17 +653,155 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552CCD6A-B613-482B-AF9E-AB5B0F15B42E}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="4" max="4" width="49.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>12345678</v>
+      </c>
+      <c r="C6">
+        <v>12345678</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="87">
+      <c r="A9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{E848326C-E1CA-48EF-8B17-F42B4B91B711}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{4DC0A7AF-38DB-478A-B3FA-CBEB0D66B4AF}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{C8E4E5E8-2092-441F-BBBA-2D9AE063E483}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{A1791070-EF24-46B2-B97A-8BA7F79B09E3}"/>
+    <hyperlink ref="A9" r:id="rId5" xr:uid="{23DB4851-3FF4-4437-91BB-3524673E50F0}"/>
+    <hyperlink ref="B9" r:id="rId6" xr:uid="{7B935EEA-2CB8-4D48-8B6E-1A0C2F51B7C3}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{6AA6D3C7-52CD-451E-8D9C-27462653A423}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9941EEDA-BEDA-4CE1-91EF-BD56BF58E9FE}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.36328125" customWidth="1"/>
+    <col min="2" max="2" width="40.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -533,8 +816,8 @@
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>24</v>
+      <c r="B2" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -547,18 +830,18 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -567,79 +850,236 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307E8AB7-7142-4B0A-9788-126B12FE2A4C}">
-  <dimension ref="A1:B2"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323277AA-92EC-41AC-A0A1-4BAC8283970E}">
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.81640625" customWidth="1"/>
+    <col min="3" max="3" width="43.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="159.5">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{A29E6A60-2CB2-4B15-A358-014F9632A6CB}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85E9C1C-BBB4-4198-80D6-0F550928EBF1}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="159.5">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="275.5">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="275.5">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="203">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="203">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="391.5">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="391.5">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel sheet updated for Register
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanja\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhavya\eclipse-workspace\bug_busters\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3C72B1-DA41-4B1A-8E65-B9AA7D562741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F6F235-10A7-41D7-A562-EF9D8952D8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
   <si>
     <t>username</t>
   </si>
@@ -207,48 +207,53 @@
     <t>password2</t>
   </si>
   <si>
-    <t xml:space="preserve">   Please fill in this field.</t>
-  </si>
-  <si>
-    <t>Numpy_Testers</t>
-  </si>
-  <si>
-    <t>Bug_Busters</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Please fill in this field.</t>
   </si>
   <si>
-    <t>*Numpy&amp;Testers*</t>
-  </si>
-  <si>
     <t>password_mismatch:The two password fields didn’t match.</t>
   </si>
   <si>
-    <t>TeamBug@busters</t>
-  </si>
-  <si>
-    <t>Team@busters</t>
-  </si>
-  <si>
-    <t>bug@12</t>
-  </si>
-  <si>
-    <t>Bug@Ninjas</t>
-  </si>
-  <si>
-    <t>Ninjas@Testers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Account Created. You are logged in as Bug@Ninjas
-</t>
+    <t>Please fill in this field.</t>
+  </si>
+  <si>
+    <t>World@Map</t>
+  </si>
+  <si>
+    <t>map_world</t>
+  </si>
+  <si>
+    <t>*World@Map*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map_world	</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map@world	</t>
+  </si>
+  <si>
+    <t>New Account Created. You are logged in as World@Map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12345678	</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> map_wr	   </t>
+  </si>
+  <si>
+    <t>map_worldmap</t>
+  </si>
+  <si>
+    <t>map_wr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +281,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -298,7 +309,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -307,6 +318,7 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -664,10 +676,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{552CCD6A-B613-482B-AF9E-AB5B0F15B42E}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -694,107 +706,117 @@
     </row>
     <row r="2" spans="1:4">
       <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6">
-        <v>12345678</v>
-      </c>
-      <c r="C6">
-        <v>12345678</v>
-      </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="87">
-      <c r="A9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>54</v>
-      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{E848326C-E1CA-48EF-8B17-F42B4B91B711}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{4DC0A7AF-38DB-478A-B3FA-CBEB0D66B4AF}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{C8E4E5E8-2092-441F-BBBA-2D9AE063E483}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{A1791070-EF24-46B2-B97A-8BA7F79B09E3}"/>
-    <hyperlink ref="A9" r:id="rId5" xr:uid="{23DB4851-3FF4-4437-91BB-3524673E50F0}"/>
-    <hyperlink ref="B9" r:id="rId6" xr:uid="{7B935EEA-2CB8-4D48-8B6E-1A0C2F51B7C3}"/>
-    <hyperlink ref="C9" r:id="rId7" xr:uid="{6AA6D3C7-52CD-451E-8D9C-27462653A423}"/>
+    <hyperlink ref="C7" r:id="rId1" display="Team@busters" xr:uid="{4DC0A7AF-38DB-478A-B3FA-CBEB0D66B4AF}"/>
+    <hyperlink ref="B8" r:id="rId2" display="bug@12" xr:uid="{C8E4E5E8-2092-441F-BBBA-2D9AE063E483}"/>
+    <hyperlink ref="C8" r:id="rId3" display="bug@12" xr:uid="{A1791070-EF24-46B2-B97A-8BA7F79B09E3}"/>
+    <hyperlink ref="A9" r:id="rId4" xr:uid="{23DB4851-3FF4-4437-91BB-3524673E50F0}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{7B935EEA-2CB8-4D48-8B6E-1A0C2F51B7C3}"/>
+    <hyperlink ref="A4" r:id="rId6" xr:uid="{A2BCCD64-FABF-4D92-A6B3-F4B459FEC929}"/>
+    <hyperlink ref="A5" r:id="rId7" xr:uid="{BE88BBC6-78C3-4C9B-9589-3584D1C4F1E9}"/>
+    <hyperlink ref="A6" r:id="rId8" xr:uid="{509FE45C-086F-4886-BB83-95B70CB59099}"/>
+    <hyperlink ref="A7" r:id="rId9" xr:uid="{41C2F899-BDDF-4D8E-AE79-C9455B698CC8}"/>
+    <hyperlink ref="A8" r:id="rId10" xr:uid="{07FD74A3-45B7-4DC8-8C6A-18CCE99A536B}"/>
+    <hyperlink ref="C9" r:id="rId11" xr:uid="{7A5B03D0-1759-4A70-8CDC-1B26349D286E}"/>
+    <hyperlink ref="B5" r:id="rId12" display="map@world_x0009__x0009_" xr:uid="{EB04038F-28B3-4677-AFC0-6CB90997C26F}"/>
+    <hyperlink ref="A3" r:id="rId13" xr:uid="{2A774A13-7AEF-4412-9E12-434E3A36D4BB}"/>
+    <hyperlink ref="B6" r:id="rId14" xr:uid="{7F18D4BF-C9C9-4276-A0E5-02848F47742B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -864,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323277AA-92EC-41AC-A0A1-4BAC8283970E}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>